<commit_message>
3 white 3 flash 4 gray done by Jim
</commit_message>
<xml_diff>
--- a/a5/flash/master.xlsx
+++ b/a5/flash/master.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="17000" tabRatio="500"/>
+    <workbookView xWindow="13940" yWindow="0" windowWidth="13940" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="8">
   <si>
     <t>PartipantID</t>
   </si>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1360,6 +1360,466 @@
       </c>
       <c r="G41">
         <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>2.8803084000000001</v>
+      </c>
+      <c r="F42">
+        <v>32.238075000000002</v>
+      </c>
+      <c r="G42">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>2.2935064000000001</v>
+      </c>
+      <c r="F43">
+        <v>59.777462</v>
+      </c>
+      <c r="G43">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>1.7930874000000001</v>
+      </c>
+      <c r="F44">
+        <v>33.340556999999997</v>
+      </c>
+      <c r="G44">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>1.6327113</v>
+      </c>
+      <c r="F45">
+        <v>72.024050000000003</v>
+      </c>
+      <c r="G45">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>1.220572</v>
+      </c>
+      <c r="F46">
+        <v>37.794609999999999</v>
+      </c>
+      <c r="G46">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>2.3356661999999999</v>
+      </c>
+      <c r="F47">
+        <v>40.077159999999999</v>
+      </c>
+      <c r="G47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>2.6220705999999998</v>
+      </c>
+      <c r="F48">
+        <v>43.968670000000003</v>
+      </c>
+      <c r="G48">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>-1.7377951</v>
+      </c>
+      <c r="F49">
+        <v>33.174827999999998</v>
+      </c>
+      <c r="G49">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>2.0890390000000001</v>
+      </c>
+      <c r="F50">
+        <v>75.870350000000002</v>
+      </c>
+      <c r="G50">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0.66562736</v>
+      </c>
+      <c r="F51">
+        <v>76.461259999999996</v>
+      </c>
+      <c r="G51">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>10</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>1.1047522999999999</v>
+      </c>
+      <c r="F52">
+        <v>62.025620000000004</v>
+      </c>
+      <c r="G52">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>-0.85019330000000004</v>
+      </c>
+      <c r="F53">
+        <v>80.42971</v>
+      </c>
+      <c r="G53">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>12</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>3.0282588000000001</v>
+      </c>
+      <c r="F54">
+        <v>28.033245000000001</v>
+      </c>
+      <c r="G54">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>13</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>1.5472918</v>
+      </c>
+      <c r="F55">
+        <v>32.79768</v>
+      </c>
+      <c r="G55">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56">
+        <v>14</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>-0.37640423000000001</v>
+      </c>
+      <c r="F56">
+        <v>24.354645000000001</v>
+      </c>
+      <c r="G56">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>15</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>1.9364768000000001</v>
+      </c>
+      <c r="F57">
+        <v>43.702697999999998</v>
+      </c>
+      <c r="G57">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <v>16</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0.67729985999999998</v>
+      </c>
+      <c r="F58">
+        <v>96.474143999999995</v>
+      </c>
+      <c r="G58">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>17</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>1.3410127000000001</v>
+      </c>
+      <c r="F59">
+        <v>62.408290000000001</v>
+      </c>
+      <c r="G59">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60">
+        <v>18</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>1.240032</v>
+      </c>
+      <c r="F60">
+        <v>87.237039999999993</v>
+      </c>
+      <c r="G60">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61">
+        <v>19</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0.23042393</v>
+      </c>
+      <c r="F61">
+        <v>73.951819999999998</v>
+      </c>
+      <c r="G61">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>